<commit_message>
replaced the harris and d'abramo 2015 data with the correct data and reran impactor flux plot appropriately, also updated usg-ground-based notes file with todos
</commit_message>
<xml_diff>
--- a/fluxes-2024-all_EDITED.xlsx
+++ b/fluxes-2024-all_EDITED.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ian\Projects\Thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90554A11-006F-4C5F-B191-E8FA5FA73B57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9429E044-AA43-4016-B80A-FA3EB0C3BA60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{95D9F6DA-D838-4D48-A421-44B65149920E}"/>
   </bookViews>
@@ -67,10 +67,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -96,9 +103,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -416,7 +425,7 @@
   <dimension ref="A1:U61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P23" sqref="P23"/>
+      <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -502,8 +511,8 @@
       <c r="K2">
         <v>7567656966424.7998</v>
       </c>
-      <c r="L2" s="1">
-        <v>2.2422E-9</v>
+      <c r="L2" s="2">
+        <v>2.2400000000000001E-9</v>
       </c>
       <c r="N2">
         <v>8.1222999999999992</v>
@@ -546,8 +555,8 @@
       <c r="K3">
         <v>3792813060042.6001</v>
       </c>
-      <c r="L3" s="1">
-        <v>4.4843999999999999E-9</v>
+      <c r="L3" s="2">
+        <v>2.2400000000000001E-9</v>
       </c>
       <c r="N3">
         <v>40.394300000000001</v>
@@ -590,8 +599,8 @@
       <c r="K4">
         <v>1900909485228.1399</v>
       </c>
-      <c r="L4" s="1">
-        <v>4.4843999999999999E-9</v>
+      <c r="L4" s="2">
+        <v>2.2400000000000001E-9</v>
       </c>
       <c r="N4">
         <v>155.69300000000001</v>
@@ -634,8 +643,8 @@
       <c r="K5">
         <v>952711566277.33398</v>
       </c>
-      <c r="L5" s="1">
-        <v>6.7266000000000003E-9</v>
+      <c r="L5" s="2">
+        <v>2.2400000000000001E-9</v>
       </c>
       <c r="N5">
         <v>537.83699999999999</v>
@@ -678,8 +687,8 @@
       <c r="K6">
         <v>477486874347.242</v>
       </c>
-      <c r="L6" s="1">
-        <v>1.1211E-8</v>
+      <c r="L6" s="2">
+        <v>4.4800000000000002E-9</v>
       </c>
       <c r="N6">
         <v>1998.15</v>
@@ -725,8 +734,8 @@
       <c r="K7">
         <v>239310325647.427</v>
       </c>
-      <c r="L7" s="1">
-        <v>1.7938000000000002E-8</v>
+      <c r="L7" s="2">
+        <v>4.4800000000000002E-9</v>
       </c>
       <c r="N7">
         <v>7984.89</v>
@@ -772,8 +781,8 @@
       <c r="K8">
         <v>119939280089.675</v>
       </c>
-      <c r="L8" s="1">
-        <v>3.3744000000000001E-8</v>
+      <c r="L8" s="2">
+        <v>6.7299999999999997E-9</v>
       </c>
       <c r="N8">
         <v>32497.7</v>
@@ -810,8 +819,8 @@
       <c r="K9">
         <v>60112035991.391296</v>
       </c>
-      <c r="L9" s="1">
-        <v>5.8385999999999998E-8</v>
+      <c r="L9" s="2">
+        <v>1.1199999999999999E-8</v>
       </c>
       <c r="N9">
         <v>118548</v>
@@ -848,8 +857,8 @@
       <c r="K10">
         <v>30127385026.228401</v>
       </c>
-      <c r="L10" s="1">
-        <v>1.2410000000000001E-7</v>
+      <c r="L10" s="2">
+        <v>1.7900000000000001E-8</v>
       </c>
       <c r="N10">
         <v>500235</v>
@@ -886,8 +895,8 @@
       <c r="K11">
         <v>15099460757.719101</v>
       </c>
-      <c r="L11" s="1">
-        <v>2.4863999999999998E-7</v>
+      <c r="L11" s="2">
+        <v>3.3699999999999997E-8</v>
       </c>
       <c r="N11">
         <v>1998520</v>
@@ -918,8 +927,8 @@
       <c r="K12">
         <v>7567656966.4247999</v>
       </c>
-      <c r="L12" s="1">
-        <v>4.4177999999999998E-7</v>
+      <c r="L12" s="2">
+        <v>5.84E-8</v>
       </c>
       <c r="N12">
         <v>8131550</v>
@@ -950,8 +959,8 @@
       <c r="K13">
         <v>3792813060.0426002</v>
       </c>
-      <c r="L13" s="1">
-        <v>7.3038000000000001E-7</v>
+      <c r="L13" s="2">
+        <v>1.24E-7</v>
       </c>
       <c r="N13">
         <v>34316128</v>
@@ -979,8 +988,8 @@
       <c r="K14">
         <v>1900909485.2281001</v>
       </c>
-      <c r="L14" s="1">
-        <v>1.1366000000000001E-6</v>
+      <c r="L14" s="2">
+        <v>2.4900000000000002E-7</v>
       </c>
       <c r="N14">
         <v>134645024</v>
@@ -1008,8 +1017,8 @@
       <c r="K15">
         <v>952711566.2773</v>
       </c>
-      <c r="L15" s="1">
-        <v>1.7803999999999999E-6</v>
+      <c r="L15" s="2">
+        <v>4.4200000000000001E-7</v>
       </c>
       <c r="N15">
         <v>537983232</v>
@@ -1037,8 +1046,8 @@
       <c r="K16">
         <v>477486874.34719998</v>
       </c>
-      <c r="L16" s="1">
-        <v>2.7306000000000002E-6</v>
+      <c r="L16" s="2">
+        <v>7.3E-7</v>
       </c>
       <c r="Q16">
         <v>438.8836</v>
@@ -1054,8 +1063,8 @@
       <c r="K17">
         <v>239310325.64739999</v>
       </c>
-      <c r="L17" s="1">
-        <v>4.3068E-6</v>
+      <c r="L17" s="2">
+        <v>1.1400000000000001E-6</v>
       </c>
       <c r="Q17">
         <v>110.68519999999999</v>
@@ -1071,8 +1080,8 @@
       <c r="K18">
         <v>119939280.0897</v>
       </c>
-      <c r="L18" s="1">
-        <v>6.3492000000000001E-6</v>
+      <c r="L18" s="2">
+        <v>1.7799999999999999E-6</v>
       </c>
       <c r="Q18">
         <v>27.910599999999999</v>
@@ -1088,8 +1097,8 @@
       <c r="K19">
         <v>60112035.991400003</v>
       </c>
-      <c r="L19" s="1">
-        <v>9.4350000000000003E-6</v>
+      <c r="L19" s="2">
+        <v>2.7300000000000001E-6</v>
       </c>
       <c r="Q19">
         <v>7.0389999999999997</v>
@@ -1105,8 +1114,8 @@
       <c r="K20">
         <v>30127385.0262</v>
       </c>
-      <c r="L20" s="1">
-        <v>1.3387000000000001E-5</v>
+      <c r="L20" s="2">
+        <v>4.3100000000000002E-6</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
@@ -1116,8 +1125,8 @@
       <c r="K21">
         <v>15099460.7577</v>
       </c>
-      <c r="L21" s="1">
-        <v>1.9069999999999999E-5</v>
+      <c r="L21" s="2">
+        <v>6.3500000000000002E-6</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
@@ -1127,8 +1136,8 @@
       <c r="K22">
         <v>7567656.9664000003</v>
       </c>
-      <c r="L22" s="1">
-        <v>2.7305999999999999E-5</v>
+      <c r="L22" s="2">
+        <v>9.4399999999999994E-6</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
@@ -1138,8 +1147,8 @@
       <c r="K23">
         <v>3792813.06</v>
       </c>
-      <c r="L23" s="1">
-        <v>3.8627999999999997E-5</v>
+      <c r="L23" s="2">
+        <v>1.34E-5</v>
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
@@ -1149,8 +1158,8 @@
       <c r="K24">
         <v>1900909.4852</v>
       </c>
-      <c r="L24" s="1">
-        <v>5.6610000000000002E-5</v>
+      <c r="L24" s="2">
+        <v>1.91E-5</v>
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
@@ -1160,8 +1169,8 @@
       <c r="K25">
         <v>952711.56629999995</v>
       </c>
-      <c r="L25" s="1">
-        <v>8.8133999999999993E-5</v>
+      <c r="L25" s="2">
+        <v>2.73E-5</v>
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
@@ -1171,8 +1180,8 @@
       <c r="K26">
         <v>477486.87430000002</v>
       </c>
-      <c r="L26" s="1">
-        <v>1.4962999999999999E-4</v>
+      <c r="L26" s="2">
+        <v>3.8600000000000003E-5</v>
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
@@ -1182,8 +1191,8 @@
       <c r="K27">
         <v>239310.32560000001</v>
       </c>
-      <c r="L27" s="1">
-        <v>2.8194E-4</v>
+      <c r="L27" s="2">
+        <v>5.66E-5</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
@@ -1193,8 +1202,8 @@
       <c r="K28">
         <v>119939.2801</v>
       </c>
-      <c r="L28" s="1">
-        <v>5.9718E-4</v>
+      <c r="L28" s="2">
+        <v>8.81E-5</v>
       </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
@@ -1204,8 +1213,8 @@
       <c r="K29">
         <v>60112.036</v>
       </c>
-      <c r="L29" s="1">
-        <v>1.403E-3</v>
+      <c r="L29" s="2">
+        <v>1.4999999999999999E-4</v>
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
@@ -1215,8 +1224,8 @@
       <c r="K30">
         <v>30127.384999999998</v>
       </c>
-      <c r="L30" s="1">
-        <v>3.2856000000000001E-3</v>
+      <c r="L30" s="2">
+        <v>2.8200000000000002E-4</v>
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
@@ -1226,16 +1235,16 @@
       <c r="K31">
         <v>15099.460800000001</v>
       </c>
-      <c r="L31" s="1">
-        <v>7.6368E-3</v>
+      <c r="L31" s="2">
+        <v>5.9699999999999998E-4</v>
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="K32">
         <v>7567.6570000000002</v>
       </c>
-      <c r="L32">
-        <v>1.6E-2</v>
+      <c r="L32" s="2">
+        <v>1.4E-3</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
@@ -1243,95 +1252,104 @@
       <c r="K33">
         <v>3792.8130999999998</v>
       </c>
-      <c r="L33">
-        <v>3.5700000000000003E-2</v>
+      <c r="L33" s="2">
+        <v>3.29E-3</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="K34">
         <v>1900.9095</v>
       </c>
-      <c r="L34">
-        <v>6.9699999999999998E-2</v>
+      <c r="L34" s="2">
+        <v>7.6400000000000001E-3</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="K35">
         <v>952.71159999999998</v>
       </c>
-      <c r="L35">
-        <v>0.1303</v>
+      <c r="L35" s="3">
+        <v>1.6E-2</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="K36">
         <v>477.48689999999999</v>
       </c>
-      <c r="L36">
-        <v>0.23089999999999999</v>
+      <c r="L36" s="3">
+        <v>3.5700000000000003E-2</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="K37">
         <v>239.31030000000001</v>
       </c>
-      <c r="L37">
-        <v>0.39739999999999998</v>
+      <c r="L37" s="3">
+        <v>6.9699999999999998E-2</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="K38">
         <v>119.9393</v>
       </c>
-      <c r="L38">
-        <v>0.57720000000000005</v>
+      <c r="L38" s="3">
+        <v>0.1303</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="K39">
         <v>60.112000000000002</v>
       </c>
-      <c r="L39">
-        <v>1.0345</v>
+      <c r="L39" s="3">
+        <v>0.23089999999999999</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="K40">
         <v>30.127400000000002</v>
       </c>
-      <c r="L40">
-        <v>1.6094999999999999</v>
+      <c r="L40" s="3">
+        <v>0.39739999999999998</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="K41">
         <v>15.099500000000001</v>
       </c>
-      <c r="L41">
-        <v>3.0413999999999999</v>
+      <c r="L41" s="3">
+        <v>0.57720000000000005</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="K42">
         <v>7.5677000000000003</v>
       </c>
-      <c r="L42">
-        <v>8.1696000000000009</v>
+      <c r="L42" s="3">
+        <v>1.0345</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="K43">
         <v>3.7928000000000002</v>
       </c>
+      <c r="L43" s="3">
+        <v>1.6094999999999999</v>
+      </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="K44">
         <v>1.9009</v>
       </c>
+      <c r="L44" s="3">
+        <v>3.0413999999999999</v>
+      </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="K45">
         <v>0.95269999999999999</v>
+      </c>
+      <c r="L45" s="3">
+        <v>8.1696000000000009</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
updated flux column headers correcting for some typos and inconsistencies
</commit_message>
<xml_diff>
--- a/fluxes-2024-all_EDITED.xlsx
+++ b/fluxes-2024-all_EDITED.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ian\Projects\Thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9429E044-AA43-4016-B80A-FA3EB0C3BA60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE76C81B-A518-4435-B605-7A358B61ED21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{95D9F6DA-D838-4D48-A421-44B65149920E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -51,16 +51,16 @@
     <t>Silber (2009)</t>
   </si>
   <si>
-    <t>Harris and d"Abramo (2015)</t>
+    <t>Harris and d'Abramo (2015)</t>
   </si>
   <si>
-    <t>Tricarirco (2016)</t>
+    <t>Tricarico (2016)</t>
   </si>
   <si>
-    <t>Schunova-Lilly(2017)</t>
+    <t>Schunova-Lilly (2017)</t>
   </si>
   <si>
-    <t>Trillings(2017)</t>
+    <t>Trillings (2017)</t>
   </si>
 </sst>
 </file>
@@ -425,7 +425,7 @@
   <dimension ref="A1:U61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M26" sqref="M26"/>
+      <selection activeCell="Q29" sqref="Q29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
updated plots, still need to fix the axis for the diameter on impactor plot and make the cdfs for D criteria...
</commit_message>
<xml_diff>
--- a/fluxes-2024-all_EDITED.xlsx
+++ b/fluxes-2024-all_EDITED.xlsx
@@ -160,10 +160,10 @@
   <dimension ref="A1:U61"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F26" activeCellId="0" sqref="F26"/>
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.28"/>
@@ -652,13 +652,10 @@
         <v>7.3025E-005</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
         <v>11.394</v>
       </c>
-      <c r="B12" s="0" t="n">
-        <v>0.1953</v>
-      </c>
       <c r="K12" s="0" t="n">
         <v>7567656966.4248</v>
       </c>
@@ -684,12 +681,9 @@
         <v>6.2114E-005</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
         <v>28.4849</v>
-      </c>
-      <c r="B13" s="0" t="n">
-        <v>0.1953</v>
       </c>
       <c r="K13" s="0" t="n">
         <v>3792813060.0426</v>

</xml_diff>